<commit_message>
Bugs, cmpany, loyalty y ultimos detalles en rutas
</commit_message>
<xml_diff>
--- a/Service.Catalog/wwwroot/layout/excel/Route/RutasFormulario.xlsx
+++ b/Service.Catalog/wwwroot/layout/excel/Route/RutasFormulario.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lapaxsis-00\source\repos\Nueva carpeta\Service.Catalog\wwwroot\layout\excel\Route\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0AF88FF-2693-44D0-9DFE-E04F5CD702AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97FE04D2-0B8F-4F35-9549-98CD5E55B8DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,8 +16,8 @@
     <sheet name="Rutas" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="Paquete" localSheetId="0">Rutas!$A$3:$C$16</definedName>
-    <definedName name="Rutas">Rutas!$C$22:$E$23</definedName>
+    <definedName name="Estudios">Rutas!$C$22:$E$23</definedName>
+    <definedName name="Rutas" localSheetId="0">Rutas!$A$3:$C$16</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -136,9 +136,6 @@
     <t>Aplicar Días</t>
   </si>
   <si>
-    <t>{{Paquete.PaqueteriaId}}</t>
-  </si>
-  <si>
     <t>{{Rutas.HoraDeRecoleccion}}</t>
   </si>
   <si>
@@ -146,6 +143,9 @@
   </si>
   <si>
     <t>{{Rutas.FormatoDeTiempoId}}</t>
+  </si>
+  <si>
+    <t>{{Rutas.PaqueteriaId}}</t>
   </si>
 </sst>
 </file>
@@ -232,14 +232,14 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -612,8 +612,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11:F11"/>
+    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -622,11 +622,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="117" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="7"/>
-      <c r="C1" s="7"/>
+      <c r="B1" s="9"/>
+      <c r="C1" s="9"/>
       <c r="D1" s="3"/>
       <c r="E1" s="3"/>
     </row>
@@ -642,7 +642,7 @@
         <v>18</v>
       </c>
       <c r="E3" s="8" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="F3" s="8"/>
     </row>
@@ -663,7 +663,7 @@
         <v>22</v>
       </c>
       <c r="E5" s="8" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F5" s="8"/>
     </row>
@@ -684,7 +684,7 @@
         <v>20</v>
       </c>
       <c r="E7" s="8" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F7" s="8"/>
     </row>
@@ -705,7 +705,7 @@
         <v>21</v>
       </c>
       <c r="E9" s="8" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F9" s="8"/>
     </row>
@@ -726,7 +726,7 @@
         <v>19</v>
       </c>
       <c r="E11" s="8" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F11" s="8"/>
     </row>
@@ -774,11 +774,11 @@
       <c r="E19" s="2"/>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C20" s="9" t="s">
+      <c r="C20" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="D20" s="9"/>
-      <c r="E20" s="9"/>
+      <c r="D20" s="7"/>
+      <c r="E20" s="7"/>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C21" s="4" t="s">
@@ -808,13 +808,6 @@
     </row>
   </sheetData>
   <mergeCells count="15">
-    <mergeCell ref="C20:E20"/>
-    <mergeCell ref="E3:F3"/>
-    <mergeCell ref="B17:C17"/>
-    <mergeCell ref="B19:C19"/>
-    <mergeCell ref="B11:C11"/>
-    <mergeCell ref="E11:F11"/>
-    <mergeCell ref="B13:C13"/>
     <mergeCell ref="A1:C1"/>
     <mergeCell ref="E5:F5"/>
     <mergeCell ref="E7:F7"/>
@@ -823,6 +816,13 @@
     <mergeCell ref="B5:C5"/>
     <mergeCell ref="B7:C7"/>
     <mergeCell ref="B9:C9"/>
+    <mergeCell ref="C20:E20"/>
+    <mergeCell ref="E3:F3"/>
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="B19:C19"/>
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="B13:C13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>

<commit_message>
Cambios en variables select, mapper, repository
</commit_message>
<xml_diff>
--- a/Service.Catalog/wwwroot/layout/excel/Route/RutasFormulario.xlsx
+++ b/Service.Catalog/wwwroot/layout/excel/Route/RutasFormulario.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lapaxsis-00\source\repos\Nueva carpeta\Service.Catalog\wwwroot\layout\excel\Route\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97FE04D2-0B8F-4F35-9549-98CD5E55B8DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E905D5B1-EE93-4188-8025-860FC6305157}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1905" yWindow="195" windowWidth="14865" windowHeight="10875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Rutas" sheetId="1" r:id="rId1"/>
@@ -100,12 +100,6 @@
     <t>{{Rutas.Nombre}}</t>
   </si>
   <si>
-    <t>{{Rutas.SucursalOrigenId}}</t>
-  </si>
-  <si>
-    <t>{{Rutas.SucursalDestinoId}}</t>
-  </si>
-  <si>
     <t>{{Rutas.Comentarios}}</t>
   </si>
   <si>
@@ -146,6 +140,12 @@
   </si>
   <si>
     <t>{{Rutas.PaqueteriaId}}</t>
+  </si>
+  <si>
+    <t>{{Rutas.SucursalOrigen}}</t>
+  </si>
+  <si>
+    <t>{{Rutas.SucursalDestino}}</t>
   </si>
 </sst>
 </file>
@@ -232,14 +232,14 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -612,8 +612,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9:C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -622,11 +622,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="117" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="9"/>
-      <c r="C1" s="9"/>
+      <c r="B1" s="7"/>
+      <c r="C1" s="7"/>
       <c r="D1" s="3"/>
       <c r="E1" s="3"/>
     </row>
@@ -639,10 +639,10 @@
       </c>
       <c r="C3" s="8"/>
       <c r="D3" s="1" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E3" s="8" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="F3" s="8"/>
     </row>
@@ -660,10 +660,10 @@
       </c>
       <c r="C5" s="8"/>
       <c r="D5" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E5" s="8" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="F5" s="8"/>
     </row>
@@ -674,17 +674,17 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B7" s="8" t="s">
-        <v>11</v>
+        <v>25</v>
       </c>
       <c r="C7" s="8"/>
       <c r="D7" s="1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="E7" s="8" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="F7" s="8"/>
     </row>
@@ -695,17 +695,17 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B9" s="8" t="s">
-        <v>12</v>
+        <v>26</v>
       </c>
       <c r="C9" s="8"/>
       <c r="D9" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="E9" s="8" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="F9" s="8"/>
     </row>
@@ -716,17 +716,17 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B11" s="8" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C11" s="8"/>
       <c r="D11" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="E11" s="8" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="F11" s="8"/>
     </row>
@@ -740,7 +740,7 @@
         <v>3</v>
       </c>
       <c r="B13" s="8" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C13" s="8"/>
     </row>
@@ -774,11 +774,11 @@
       <c r="E19" s="2"/>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C20" s="7" t="s">
+      <c r="C20" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="D20" s="7"/>
-      <c r="E20" s="7"/>
+      <c r="D20" s="9"/>
+      <c r="E20" s="9"/>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C21" s="4" t="s">
@@ -808,6 +808,13 @@
     </row>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="C20:E20"/>
+    <mergeCell ref="E3:F3"/>
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="B19:C19"/>
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="B13:C13"/>
     <mergeCell ref="A1:C1"/>
     <mergeCell ref="E5:F5"/>
     <mergeCell ref="E7:F7"/>
@@ -816,13 +823,6 @@
     <mergeCell ref="B5:C5"/>
     <mergeCell ref="B7:C7"/>
     <mergeCell ref="B9:C9"/>
-    <mergeCell ref="C20:E20"/>
-    <mergeCell ref="E3:F3"/>
-    <mergeCell ref="B17:C17"/>
-    <mergeCell ref="B19:C19"/>
-    <mergeCell ref="B11:C11"/>
-    <mergeCell ref="E11:F11"/>
-    <mergeCell ref="B13:C13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>